<commit_message>
"one for all function for correction"
</commit_message>
<xml_diff>
--- a/Kres/test/_svod_2312.xlsx
+++ b/Kres/test/_svod_2312.xlsx
@@ -275,9 +275,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left/>
+        <right/>
         <top style="thin">
           <color theme="5"/>
         </top>
+        <bottom/>
+        <diagonal/>
       </border>
     </dxf>
     <dxf>
@@ -333,6 +337,7 @@
           <color theme="7"/>
         </top>
         <bottom/>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -345,6 +350,7 @@
           <color theme="7"/>
         </top>
         <bottom/>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -357,6 +363,7 @@
           <color theme="7"/>
         </top>
         <bottom/>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -369,6 +376,7 @@
           <color theme="7"/>
         </top>
         <bottom/>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -381,6 +389,7 @@
           <color theme="7"/>
         </top>
         <bottom/>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -393,6 +402,7 @@
           <color theme="7"/>
         </top>
         <bottom/>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -405,6 +415,7 @@
           <color theme="7"/>
         </top>
         <bottom/>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -417,6 +428,7 @@
           <color theme="7"/>
         </top>
         <bottom/>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -429,6 +441,7 @@
           <color theme="7"/>
         </top>
         <bottom/>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -441,6 +454,7 @@
           <color theme="7"/>
         </top>
         <bottom/>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -453,6 +467,7 @@
           <color theme="7"/>
         </top>
         <bottom/>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -465,6 +480,7 @@
           <color theme="7"/>
         </top>
         <bottom/>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -497,6 +513,7 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -526,6 +543,7 @@
         </right>
         <top/>
         <bottom/>
+        <diagonal/>
       </border>
     </dxf>
   </dxfs>
@@ -2155,7 +2173,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>12.01</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="N3" t="inlineStr"/>
@@ -2222,7 +2240,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>1.20</t>
+          <t>1.21</t>
         </is>
       </c>
       <c r="N4" t="inlineStr"/>

</xml_diff>